<commit_message>
Added more robut error handling to catch common numerical issues
</commit_message>
<xml_diff>
--- a/Financial Modelling Prep Library/Company Financial Data/EOG/annual/cash_flow_statements.xlsx
+++ b/Financial Modelling Prep Library/Company Financial Data/EOG/annual/cash_flow_statements.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="163">
   <si>
     <t>date</t>
   </si>
@@ -139,30 +139,6 @@
     <t>index</t>
   </si>
   <si>
-    <t>EOG-FY-1994</t>
-  </si>
-  <si>
-    <t>EOG-FY-1995</t>
-  </si>
-  <si>
-    <t>EOG-FY-1996</t>
-  </si>
-  <si>
-    <t>EOG-FY-1997</t>
-  </si>
-  <si>
-    <t>EOG-FY-1998</t>
-  </si>
-  <si>
-    <t>EOG-FY-1999</t>
-  </si>
-  <si>
-    <t>EOG-FY-2000</t>
-  </si>
-  <si>
-    <t>EOG-FY-2001</t>
-  </si>
-  <si>
     <t>EOG-FY-2002</t>
   </si>
   <si>
@@ -232,30 +208,6 @@
     <t>0000821189</t>
   </si>
   <si>
-    <t>1994-12-31</t>
-  </si>
-  <si>
-    <t>1995-12-31</t>
-  </si>
-  <si>
-    <t>1996-12-31</t>
-  </si>
-  <si>
-    <t>1997-12-31</t>
-  </si>
-  <si>
-    <t>1998-12-31</t>
-  </si>
-  <si>
-    <t>2000-03-08</t>
-  </si>
-  <si>
-    <t>2001-03-23</t>
-  </si>
-  <si>
-    <t>2001-12-31</t>
-  </si>
-  <si>
     <t>2002-12-31</t>
   </si>
   <si>
@@ -316,30 +268,6 @@
     <t>2022-02-24</t>
   </si>
   <si>
-    <t>1994-12-30 19:00:00</t>
-  </si>
-  <si>
-    <t>1995-12-30 19:00:00</t>
-  </si>
-  <si>
-    <t>1996-12-30 19:00:00</t>
-  </si>
-  <si>
-    <t>1997-12-30 19:00:00</t>
-  </si>
-  <si>
-    <t>1998-12-30 19:00:00</t>
-  </si>
-  <si>
-    <t>2000-03-08 00:00:00</t>
-  </si>
-  <si>
-    <t>2001-03-23 00:00:00</t>
-  </si>
-  <si>
-    <t>2002-03-20 00:00:00</t>
-  </si>
-  <si>
     <t>2003-03-13 16:50:47</t>
   </si>
   <si>
@@ -400,30 +328,6 @@
     <t>2022-02-24 16:51:16</t>
   </si>
   <si>
-    <t>1994</t>
-  </si>
-  <si>
-    <t>1995</t>
-  </si>
-  <si>
-    <t>1996</t>
-  </si>
-  <si>
-    <t>1997</t>
-  </si>
-  <si>
-    <t>1998</t>
-  </si>
-  <si>
-    <t>1999</t>
-  </si>
-  <si>
-    <t>2000</t>
-  </si>
-  <si>
-    <t>2001</t>
-  </si>
-  <si>
     <t>2002</t>
   </si>
   <si>
@@ -487,12 +391,6 @@
     <t>FY</t>
   </si>
   <si>
-    <t>https://www.sec.gov/Archives/edgar/data/821189/0000950129-00-001017-index.html</t>
-  </si>
-  <si>
-    <t>https://www.sec.gov/Archives/edgar/data/821189/000082118901500007/0000821189-01-500007-index.htm</t>
-  </si>
-  <si>
     <t>https://www.sec.gov/Archives/edgar/data/821189/000082118904000070/0000821189-04-000070-index.htm</t>
   </si>
   <si>
@@ -548,12 +446,6 @@
   </si>
   <si>
     <t>https://www.sec.gov/Archives/edgar/data/821189/000082118922000017/0000821189-22-000017-index.htm</t>
-  </si>
-  <si>
-    <t>https://www.sec.gov/Archives/edgar/data/821189/000095012900001017/</t>
-  </si>
-  <si>
-    <t>https://www.sec.gov/Archives/edgar/data/821189/000082118901500007/form10k2000.txt</t>
   </si>
   <si>
     <t>https://www.sec.gov/Archives/edgar/data/821189/000082118904000070/eog10-k03.txt</t>
@@ -985,7 +877,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AO29"/>
+  <dimension ref="A1:AO21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1121,64 +1013,64 @@
         <v>41</v>
       </c>
       <c r="B2" s="2">
-        <v>34699</v>
+        <v>37621</v>
       </c>
       <c r="C2" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="D2" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="E2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="F2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="G2" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="H2" t="s">
-        <v>128</v>
+        <v>104</v>
       </c>
       <c r="I2" t="s">
-        <v>156</v>
+        <v>124</v>
       </c>
       <c r="J2">
-        <v>148000000</v>
+        <v>87173000</v>
       </c>
       <c r="K2">
-        <v>242200000</v>
+        <v>398036000</v>
       </c>
       <c r="L2">
-        <v>1800000</v>
+        <v>82179000</v>
       </c>
       <c r="M2">
         <v>0</v>
       </c>
       <c r="N2">
-        <v>-28800000</v>
+        <v>-114717000</v>
       </c>
       <c r="O2">
         <v>0</v>
       </c>
       <c r="P2">
-        <v>-2200000</v>
+        <v>-57000</v>
       </c>
       <c r="Q2">
         <v>0</v>
       </c>
       <c r="R2">
-        <v>-8200000</v>
+        <v>42782000</v>
       </c>
       <c r="S2">
-        <v>62700000</v>
+        <v>215899000</v>
       </c>
       <c r="T2">
-        <v>425900000</v>
+        <v>668570000</v>
       </c>
       <c r="U2">
-        <v>-442100000</v>
+        <v>-714127000</v>
       </c>
       <c r="V2">
         <v>0</v>
@@ -1190,49 +1082,49 @@
         <v>0</v>
       </c>
       <c r="Y2">
-        <v>-52700000</v>
+        <v>-158411000</v>
       </c>
       <c r="Z2">
-        <v>-494800000</v>
+        <v>-872538000</v>
       </c>
       <c r="AA2">
         <v>0</v>
       </c>
       <c r="AB2">
-        <v>4100000</v>
+        <v>17339000</v>
       </c>
       <c r="AC2">
-        <v>-14100000</v>
+        <v>-63038000</v>
       </c>
       <c r="AD2">
-        <v>-19200000</v>
+        <v>-29152000</v>
       </c>
       <c r="AE2">
-        <v>800000</v>
+        <v>286155000</v>
       </c>
       <c r="AF2">
-        <v>-28400000</v>
+        <v>211304000</v>
       </c>
       <c r="AG2">
         <v>0</v>
       </c>
       <c r="AH2">
-        <v>0</v>
+        <v>7336000</v>
       </c>
       <c r="AI2">
-        <v>0</v>
+        <v>9848000</v>
       </c>
       <c r="AJ2">
-        <v>103100000</v>
+        <v>2512000</v>
       </c>
       <c r="AK2">
-        <v>425900000</v>
+        <v>668570000</v>
       </c>
       <c r="AL2">
-        <v>-442100000</v>
+        <v>-714127000</v>
       </c>
       <c r="AM2">
-        <v>-16200000</v>
+        <v>-45557000</v>
       </c>
     </row>
     <row r="3" spans="1:41">
@@ -1240,64 +1132,64 @@
         <v>42</v>
       </c>
       <c r="B3" s="2">
-        <v>35064</v>
+        <v>37986</v>
       </c>
       <c r="C3" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="D3" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="E3" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="F3" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="G3" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="H3" t="s">
-        <v>129</v>
+        <v>105</v>
       </c>
       <c r="I3" t="s">
-        <v>156</v>
+        <v>124</v>
       </c>
       <c r="J3">
-        <v>142100000</v>
+        <v>430145000</v>
       </c>
       <c r="K3">
-        <v>216000000</v>
+        <v>441843000</v>
       </c>
       <c r="L3">
-        <v>45200000</v>
+        <v>191726000</v>
       </c>
       <c r="M3">
         <v>0</v>
       </c>
       <c r="N3">
-        <v>-7500000</v>
+        <v>9568000</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3">
-        <v>4000000</v>
+        <v>-2994000</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>48500000</v>
+        <v>-35928000</v>
       </c>
       <c r="S3">
-        <v>-60400000</v>
+        <v>247019000</v>
       </c>
       <c r="T3">
-        <v>335400000</v>
+        <v>1320301000</v>
       </c>
       <c r="U3">
-        <v>-445000000</v>
+        <v>-1204383000</v>
       </c>
       <c r="V3">
         <v>0</v>
@@ -1309,49 +1201,55 @@
         <v>0</v>
       </c>
       <c r="Y3">
-        <v>53700000</v>
+        <v>-64127000</v>
       </c>
       <c r="Z3">
-        <v>-391300000</v>
+        <v>-1268510000</v>
       </c>
       <c r="AA3">
         <v>0</v>
       </c>
       <c r="AB3">
-        <v>10300000</v>
+        <v>35138000</v>
       </c>
       <c r="AC3">
-        <v>-17900000</v>
+        <v>-21295000</v>
       </c>
       <c r="AD3">
-        <v>-19200000</v>
+        <v>-31294000</v>
       </c>
       <c r="AE3">
-        <v>100000000</v>
+        <v>-39745000</v>
       </c>
       <c r="AF3">
-        <v>73200000</v>
+        <v>-57196000</v>
       </c>
       <c r="AG3">
         <v>0</v>
       </c>
       <c r="AH3">
-        <v>0</v>
+        <v>-5405000</v>
       </c>
       <c r="AI3">
-        <v>0</v>
+        <v>4443000</v>
       </c>
       <c r="AJ3">
-        <v>5800000</v>
+        <v>9848000</v>
       </c>
       <c r="AK3">
-        <v>335400000</v>
+        <v>1320301000</v>
       </c>
       <c r="AL3">
-        <v>-445000000</v>
+        <v>-1204383000</v>
       </c>
       <c r="AM3">
-        <v>-109600000</v>
+        <v>115918000</v>
+      </c>
+      <c r="AN3" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="AO3" s="3" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:41">
@@ -1359,64 +1257,64 @@
         <v>43</v>
       </c>
       <c r="B4" s="2">
-        <v>35430</v>
+        <v>38352</v>
       </c>
       <c r="C4" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="D4" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="E4" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="F4" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="G4" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="H4" t="s">
-        <v>130</v>
+        <v>106</v>
       </c>
       <c r="I4" t="s">
-        <v>156</v>
+        <v>124</v>
       </c>
       <c r="J4">
-        <v>140000000</v>
+        <v>624855000</v>
       </c>
       <c r="K4">
-        <v>251300000</v>
+        <v>504403000</v>
       </c>
       <c r="L4">
-        <v>2300000</v>
+        <v>204231000</v>
       </c>
       <c r="M4">
         <v>0</v>
       </c>
       <c r="N4">
-        <v>-39200000</v>
+        <v>-44929000</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4">
-        <v>-9000000</v>
+        <v>-17898000</v>
       </c>
       <c r="Q4">
         <v>0</v>
       </c>
       <c r="R4">
-        <v>8500000</v>
+        <v>-28381000</v>
       </c>
       <c r="S4">
-        <v>10700000</v>
+        <v>155787000</v>
       </c>
       <c r="T4">
-        <v>365100000</v>
+        <v>1444347000</v>
       </c>
       <c r="U4">
-        <v>-539300000</v>
+        <v>-1416684000</v>
       </c>
       <c r="V4">
         <v>0</v>
@@ -1428,49 +1326,55 @@
         <v>0</v>
       </c>
       <c r="Y4">
-        <v>27700000</v>
+        <v>19776000</v>
       </c>
       <c r="Z4">
-        <v>-511600000</v>
+        <v>-1396908000</v>
       </c>
       <c r="AA4">
         <v>0</v>
       </c>
       <c r="AB4">
-        <v>22200000</v>
+        <v>75510000</v>
       </c>
       <c r="AC4">
-        <v>-43500000</v>
+        <v>-50000000</v>
       </c>
       <c r="AD4">
-        <v>-19200000</v>
+        <v>-37595000</v>
       </c>
       <c r="AE4">
-        <v>171600000</v>
+        <v>-31153000</v>
       </c>
       <c r="AF4">
-        <v>131100000</v>
+        <v>-43238000</v>
       </c>
       <c r="AG4">
-        <v>0</v>
+        <v>12336000</v>
       </c>
       <c r="AH4">
-        <v>0</v>
+        <v>16537000</v>
       </c>
       <c r="AI4">
-        <v>0</v>
+        <v>20980000</v>
       </c>
       <c r="AJ4">
-        <v>23000000</v>
+        <v>4443000</v>
       </c>
       <c r="AK4">
-        <v>365100000</v>
+        <v>1444347000</v>
       </c>
       <c r="AL4">
-        <v>-539300000</v>
+        <v>-1416684000</v>
       </c>
       <c r="AM4">
-        <v>-174200000</v>
+        <v>27663000</v>
+      </c>
+      <c r="AN4" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="AO4" s="3" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="5" spans="1:41">
@@ -1478,64 +1382,64 @@
         <v>44</v>
       </c>
       <c r="B5" s="2">
-        <v>35795</v>
+        <v>38717</v>
       </c>
       <c r="C5" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="D5" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="E5" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="F5" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="G5" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="H5" t="s">
-        <v>131</v>
+        <v>107</v>
       </c>
       <c r="I5" t="s">
-        <v>156</v>
+        <v>124</v>
       </c>
       <c r="J5">
-        <v>122000000</v>
+        <v>1259576000</v>
       </c>
       <c r="K5">
-        <v>278200000</v>
+        <v>654258000</v>
       </c>
       <c r="L5">
-        <v>16700000</v>
+        <v>270291000</v>
       </c>
       <c r="M5">
         <v>0</v>
       </c>
       <c r="N5">
-        <v>48700000</v>
+        <v>-13640000</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5">
-        <v>-11300000</v>
+        <v>-23085000</v>
       </c>
       <c r="Q5">
         <v>0</v>
       </c>
       <c r="R5">
-        <v>-9000000</v>
+        <v>-10347000</v>
       </c>
       <c r="S5">
-        <v>65300000</v>
+        <v>198941000</v>
       </c>
       <c r="T5">
-        <v>530900000</v>
+        <v>2369426000</v>
       </c>
       <c r="U5">
-        <v>-626200000</v>
+        <v>-1724763000</v>
       </c>
       <c r="V5">
         <v>0</v>
@@ -1547,49 +1451,55 @@
         <v>0</v>
       </c>
       <c r="Y5">
-        <v>-70900000</v>
+        <v>46655000</v>
       </c>
       <c r="Z5">
-        <v>-697100000</v>
+        <v>-1678108000</v>
       </c>
       <c r="AA5">
         <v>0</v>
       </c>
       <c r="AB5">
-        <v>5100000</v>
+        <v>64668000</v>
       </c>
       <c r="AC5">
-        <v>-99300000</v>
+        <v>0</v>
       </c>
       <c r="AD5">
-        <v>-18900000</v>
+        <v>-42986000</v>
       </c>
       <c r="AE5">
-        <v>281000000</v>
+        <v>-93992000</v>
       </c>
       <c r="AF5">
-        <v>167900000</v>
+        <v>-72310000</v>
       </c>
       <c r="AG5">
-        <v>0</v>
+        <v>3823000</v>
       </c>
       <c r="AH5">
-        <v>0</v>
+        <v>622831000</v>
       </c>
       <c r="AI5">
-        <v>0</v>
+        <v>643811000</v>
       </c>
       <c r="AJ5">
-        <v>7600000</v>
+        <v>20980000</v>
       </c>
       <c r="AK5">
-        <v>530900000</v>
+        <v>2369426000</v>
       </c>
       <c r="AL5">
-        <v>-626200000</v>
+        <v>-1724763000</v>
       </c>
       <c r="AM5">
-        <v>-95300000</v>
+        <v>644663000</v>
+      </c>
+      <c r="AN5" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="AO5" s="3" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:41">
@@ -1597,64 +1507,64 @@
         <v>45</v>
       </c>
       <c r="B6" s="2">
-        <v>36160</v>
+        <v>39082</v>
       </c>
       <c r="C6" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="D6" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="E6" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="F6" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="G6" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="H6" t="s">
-        <v>132</v>
+        <v>108</v>
       </c>
       <c r="I6" t="s">
-        <v>156</v>
+        <v>124</v>
       </c>
       <c r="J6">
-        <v>56200000</v>
+        <v>1299885000</v>
       </c>
       <c r="K6">
-        <v>315100000</v>
+        <v>817089000</v>
       </c>
       <c r="L6">
-        <v>-26800000</v>
+        <v>385842000</v>
       </c>
       <c r="M6">
         <v>0</v>
       </c>
       <c r="N6">
-        <v>-46400000</v>
+        <v>-45032000</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6">
-        <v>-7500000</v>
+        <v>-50370000</v>
       </c>
       <c r="Q6">
         <v>0</v>
       </c>
       <c r="R6">
-        <v>-16200000</v>
+        <v>-120255000</v>
       </c>
       <c r="S6">
-        <v>105500000</v>
+        <v>120769000</v>
       </c>
       <c r="T6">
-        <v>403600000</v>
+        <v>2578553000</v>
       </c>
       <c r="U6">
-        <v>-690400000</v>
+        <v>-2819230000</v>
       </c>
       <c r="V6">
         <v>0</v>
@@ -1666,49 +1576,55 @@
         <v>0</v>
       </c>
       <c r="Y6">
-        <v>-69200000</v>
+        <v>108857000</v>
       </c>
       <c r="Z6">
-        <v>-759600000</v>
+        <v>-2710373000</v>
       </c>
       <c r="AA6">
         <v>0</v>
       </c>
       <c r="AB6">
-        <v>2900000</v>
+        <v>36033000</v>
       </c>
       <c r="AC6">
-        <v>-25900000</v>
+        <v>-50199000</v>
       </c>
       <c r="AD6">
-        <v>-18500000</v>
+        <v>-60443000</v>
       </c>
       <c r="AE6">
-        <v>394500000</v>
+        <v>-224273000</v>
       </c>
       <c r="AF6">
-        <v>353000000</v>
+        <v>-298882000</v>
       </c>
       <c r="AG6">
-        <v>0</v>
+        <v>5146000</v>
       </c>
       <c r="AH6">
-        <v>0</v>
+        <v>-425556000</v>
       </c>
       <c r="AI6">
-        <v>0</v>
+        <v>218255000</v>
       </c>
       <c r="AJ6">
-        <v>9300000</v>
+        <v>643811000</v>
       </c>
       <c r="AK6">
-        <v>403600000</v>
+        <v>2578553000</v>
       </c>
       <c r="AL6">
-        <v>-690400000</v>
+        <v>-2819230000</v>
       </c>
       <c r="AM6">
-        <v>-286800000</v>
+        <v>-240677000</v>
+      </c>
+      <c r="AN6" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="AO6" s="3" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="7" spans="1:41">
@@ -1716,64 +1632,64 @@
         <v>46</v>
       </c>
       <c r="B7" s="2">
-        <v>36525</v>
+        <v>39447</v>
       </c>
       <c r="C7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F7" t="s">
         <v>69</v>
       </c>
-      <c r="D7" t="s">
-        <v>70</v>
-      </c>
-      <c r="E7" t="s">
-        <v>71</v>
-      </c>
-      <c r="F7" t="s">
-        <v>77</v>
-      </c>
       <c r="G7" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="H7" t="s">
-        <v>133</v>
+        <v>109</v>
       </c>
       <c r="I7" t="s">
-        <v>156</v>
+        <v>124</v>
       </c>
       <c r="J7">
-        <v>569100000</v>
+        <v>1089918000</v>
       </c>
       <c r="K7">
-        <v>459900000</v>
+        <v>1065545000</v>
       </c>
       <c r="L7">
-        <v>-26300000</v>
+        <v>426827000</v>
       </c>
       <c r="M7">
         <v>0</v>
       </c>
       <c r="N7">
-        <v>-24200000</v>
+        <v>109526000</v>
       </c>
       <c r="O7">
         <v>0</v>
       </c>
       <c r="P7">
-        <v>5200000</v>
+        <v>9638000</v>
       </c>
       <c r="Q7">
         <v>0</v>
       </c>
       <c r="R7">
-        <v>-18100000</v>
+        <v>-3440000</v>
       </c>
       <c r="S7">
-        <v>-536400000</v>
+        <v>201549000</v>
       </c>
       <c r="T7">
-        <v>442100000</v>
+        <v>2893365000</v>
       </c>
       <c r="U7">
-        <v>-402800000</v>
+        <v>-3679062000</v>
       </c>
       <c r="V7">
         <v>0</v>
@@ -1785,55 +1701,55 @@
         <v>0</v>
       </c>
       <c r="Y7">
-        <v>39400000</v>
+        <v>223288000</v>
       </c>
       <c r="Z7">
-        <v>-363400000</v>
+        <v>-3455774000</v>
       </c>
       <c r="AA7">
         <v>0</v>
       </c>
       <c r="AB7">
-        <v>739800000</v>
+        <v>55320000</v>
       </c>
       <c r="AC7">
-        <v>-2100000</v>
+        <v>-51197000</v>
       </c>
       <c r="AD7">
-        <v>-17400000</v>
+        <v>-84020000</v>
       </c>
       <c r="AE7">
-        <v>-780500000</v>
+        <v>473620000</v>
       </c>
       <c r="AF7">
-        <v>-60200000</v>
+        <v>393723000</v>
       </c>
       <c r="AG7">
-        <v>0</v>
+        <v>4662000</v>
       </c>
       <c r="AH7">
-        <v>18500000</v>
+        <v>-164024000</v>
       </c>
       <c r="AI7">
-        <v>24800000</v>
+        <v>54231000</v>
       </c>
       <c r="AJ7">
-        <v>6300000</v>
+        <v>218255000</v>
       </c>
       <c r="AK7">
-        <v>442100000</v>
+        <v>2893365000</v>
       </c>
       <c r="AL7">
-        <v>-402800000</v>
+        <v>-3679062000</v>
       </c>
       <c r="AM7">
-        <v>39300000</v>
+        <v>-785697000</v>
       </c>
       <c r="AN7" s="3" t="s">
-        <v>157</v>
+        <v>129</v>
       </c>
       <c r="AO7" s="3" t="s">
-        <v>178</v>
+        <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:41">
@@ -1841,64 +1757,64 @@
         <v>47</v>
       </c>
       <c r="B8" s="2">
-        <v>36891</v>
+        <v>39813</v>
       </c>
       <c r="C8" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="D8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" t="s">
+        <v>63</v>
+      </c>
+      <c r="F8" t="s">
         <v>70</v>
       </c>
-      <c r="E8" t="s">
-        <v>71</v>
-      </c>
-      <c r="F8" t="s">
-        <v>78</v>
-      </c>
       <c r="G8" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="H8" t="s">
-        <v>134</v>
+        <v>110</v>
       </c>
       <c r="I8" t="s">
-        <v>156</v>
+        <v>124</v>
       </c>
       <c r="J8">
-        <v>396931000</v>
+        <v>2436919000</v>
       </c>
       <c r="K8">
-        <v>370026000</v>
+        <v>1326875000</v>
       </c>
       <c r="L8">
-        <v>97729000</v>
+        <v>1133630000</v>
       </c>
       <c r="M8">
         <v>0</v>
       </c>
       <c r="N8">
-        <v>-25491000</v>
+        <v>97736000</v>
       </c>
       <c r="O8">
         <v>0</v>
       </c>
       <c r="P8">
-        <v>2345000</v>
+        <v>-92049000</v>
       </c>
       <c r="Q8">
         <v>0</v>
       </c>
       <c r="R8">
-        <v>24749000</v>
+        <v>-1654000</v>
       </c>
       <c r="S8">
-        <v>128215000</v>
+        <v>-361911000</v>
       </c>
       <c r="T8">
-        <v>967410000</v>
+        <v>4633249000</v>
       </c>
       <c r="U8">
-        <v>-602638000</v>
+        <v>-5195471000</v>
       </c>
       <c r="V8">
         <v>0</v>
@@ -1910,55 +1826,55 @@
         <v>0</v>
       </c>
       <c r="Y8">
-        <v>-64523000</v>
+        <v>228953000</v>
       </c>
       <c r="Z8">
-        <v>-667161000</v>
+        <v>-4966518000</v>
       </c>
       <c r="AA8">
         <v>0</v>
       </c>
       <c r="AB8">
-        <v>127090000</v>
+        <v>72572000</v>
       </c>
       <c r="AC8">
-        <v>-272723000</v>
+        <v>-23229000</v>
       </c>
       <c r="AD8">
-        <v>-26071000</v>
+        <v>-115204000</v>
       </c>
       <c r="AE8">
-        <v>-133229000</v>
+        <v>710966000</v>
       </c>
       <c r="AF8">
-        <v>-304933000</v>
+        <v>645105000</v>
       </c>
       <c r="AG8">
-        <v>0</v>
+        <v>-34756000</v>
       </c>
       <c r="AH8">
-        <v>-4684000</v>
+        <v>277080000</v>
       </c>
       <c r="AI8">
-        <v>20152000</v>
+        <v>331311000</v>
       </c>
       <c r="AJ8">
-        <v>24836000</v>
+        <v>54231000</v>
       </c>
       <c r="AK8">
-        <v>967410000</v>
+        <v>4633249000</v>
       </c>
       <c r="AL8">
-        <v>-602638000</v>
+        <v>-5195471000</v>
       </c>
       <c r="AM8">
-        <v>364772000</v>
+        <v>-562222000</v>
       </c>
       <c r="AN8" s="3" t="s">
-        <v>158</v>
+        <v>130</v>
       </c>
       <c r="AO8" s="3" t="s">
-        <v>179</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:41">
@@ -1966,118 +1882,124 @@
         <v>48</v>
       </c>
       <c r="B9" s="2">
-        <v>37256</v>
+        <v>40178</v>
       </c>
       <c r="C9" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="D9" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="E9" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9" t="s">
         <v>71</v>
       </c>
-      <c r="F9" t="s">
-        <v>79</v>
-      </c>
       <c r="G9" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="H9" t="s">
-        <v>135</v>
+        <v>111</v>
       </c>
       <c r="I9" t="s">
-        <v>156</v>
+        <v>124</v>
       </c>
       <c r="J9">
-        <v>398616000</v>
+        <v>546627000</v>
       </c>
       <c r="K9">
-        <v>392399000</v>
+        <v>0</v>
       </c>
       <c r="L9">
-        <v>164945000</v>
+        <v>174392000</v>
       </c>
       <c r="M9">
-        <v>0</v>
+        <v>95180000</v>
       </c>
       <c r="N9">
-        <v>24450000</v>
+        <v>-178420000</v>
       </c>
       <c r="O9">
-        <v>0</v>
+        <v>-47818000</v>
       </c>
       <c r="P9">
-        <v>-2248000</v>
+        <v>-50146000</v>
       </c>
       <c r="Q9">
-        <v>0</v>
+        <v>-153565000</v>
       </c>
       <c r="R9">
-        <v>-50547000</v>
+        <v>-17820000</v>
       </c>
       <c r="S9">
-        <v>217017000</v>
+        <v>2284660000</v>
       </c>
       <c r="T9">
-        <v>1197427000</v>
+        <v>2922439000</v>
       </c>
       <c r="U9">
-        <v>-974016000</v>
+        <v>-3503009000</v>
       </c>
       <c r="V9">
         <v>0</v>
       </c>
       <c r="W9">
-        <v>0</v>
+        <v>-118221000</v>
       </c>
       <c r="X9">
         <v>0</v>
       </c>
       <c r="Y9">
-        <v>-114039000</v>
+        <v>206679000</v>
       </c>
       <c r="Z9">
-        <v>-1088055000</v>
+        <v>-3414551000</v>
       </c>
       <c r="AA9">
         <v>0</v>
       </c>
       <c r="AB9">
-        <v>30805000</v>
+        <v>0</v>
       </c>
       <c r="AC9">
-        <v>-126769000</v>
+        <v>-10986000</v>
       </c>
       <c r="AD9">
-        <v>-28580000</v>
+        <v>-142260000</v>
       </c>
       <c r="AE9">
-        <v>-2468000</v>
+        <v>987408000</v>
       </c>
       <c r="AF9">
-        <v>-127012000</v>
+        <v>834162000</v>
       </c>
       <c r="AG9">
-        <v>0</v>
+        <v>12390000</v>
       </c>
       <c r="AH9">
-        <v>-17640000</v>
+        <v>354440000</v>
       </c>
       <c r="AI9">
-        <v>2512000</v>
+        <v>685751000</v>
       </c>
       <c r="AJ9">
-        <v>20152000</v>
+        <v>331311000</v>
       </c>
       <c r="AK9">
-        <v>1197427000</v>
+        <v>2922439000</v>
       </c>
       <c r="AL9">
-        <v>-974016000</v>
+        <v>-3503009000</v>
       </c>
       <c r="AM9">
-        <v>223411000</v>
+        <v>-580570000</v>
+      </c>
+      <c r="AN9" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="AO9" s="3" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="10" spans="1:41">
@@ -2085,67 +2007,67 @@
         <v>49</v>
       </c>
       <c r="B10" s="2">
-        <v>37621</v>
+        <v>40543</v>
       </c>
       <c r="C10" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="D10" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="E10" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="F10" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="G10" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="H10" t="s">
-        <v>136</v>
+        <v>112</v>
       </c>
       <c r="I10" t="s">
-        <v>156</v>
+        <v>124</v>
       </c>
       <c r="J10">
-        <v>87173000</v>
+        <v>160654000</v>
       </c>
       <c r="K10">
-        <v>398036000</v>
+        <v>0</v>
       </c>
       <c r="L10">
-        <v>82179000</v>
+        <v>76245000</v>
       </c>
       <c r="M10">
-        <v>0</v>
+        <v>107378000</v>
       </c>
       <c r="N10">
-        <v>-114717000</v>
+        <v>-131122000</v>
       </c>
       <c r="O10">
-        <v>0</v>
+        <v>-339126000</v>
       </c>
       <c r="P10">
-        <v>-57000</v>
+        <v>-171791000</v>
       </c>
       <c r="Q10">
-        <v>0</v>
+        <v>654688000</v>
       </c>
       <c r="R10">
-        <v>42782000</v>
+        <v>-221795000</v>
       </c>
       <c r="S10">
-        <v>215899000</v>
+        <v>2495447000</v>
       </c>
       <c r="T10">
-        <v>668570000</v>
+        <v>2708602000</v>
       </c>
       <c r="U10">
-        <v>-714127000</v>
+        <v>-5581382000</v>
       </c>
       <c r="V10">
-        <v>0</v>
+        <v>-210000000</v>
       </c>
       <c r="W10">
         <v>0</v>
@@ -2154,49 +2076,55 @@
         <v>0</v>
       </c>
       <c r="Y10">
-        <v>-158411000</v>
+        <v>888608000</v>
       </c>
       <c r="Z10">
-        <v>-872538000</v>
+        <v>-4902774000</v>
       </c>
       <c r="AA10">
-        <v>0</v>
+        <v>-45300000</v>
       </c>
       <c r="AB10">
-        <v>17339000</v>
+        <v>0</v>
       </c>
       <c r="AC10">
-        <v>-63038000</v>
+        <v>-11295000</v>
       </c>
       <c r="AD10">
-        <v>-29152000</v>
+        <v>-153240000</v>
       </c>
       <c r="AE10">
-        <v>286155000</v>
+        <v>2513254000</v>
       </c>
       <c r="AF10">
-        <v>211304000</v>
+        <v>2303419000</v>
       </c>
       <c r="AG10">
-        <v>0</v>
+        <v>-6145000</v>
       </c>
       <c r="AH10">
-        <v>7336000</v>
+        <v>103102000</v>
       </c>
       <c r="AI10">
-        <v>9848000</v>
+        <v>788853000</v>
       </c>
       <c r="AJ10">
-        <v>2512000</v>
+        <v>685751000</v>
       </c>
       <c r="AK10">
-        <v>668570000</v>
+        <v>2708602000</v>
       </c>
       <c r="AL10">
-        <v>-714127000</v>
+        <v>-5581382000</v>
       </c>
       <c r="AM10">
-        <v>-45557000</v>
+        <v>-2872780000</v>
+      </c>
+      <c r="AN10" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="AO10" s="3" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="11" spans="1:41">
@@ -2204,124 +2132,124 @@
         <v>50</v>
       </c>
       <c r="B11" s="2">
-        <v>37986</v>
+        <v>40907</v>
       </c>
       <c r="C11" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="D11" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="E11" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="F11" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="G11" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="H11" t="s">
-        <v>137</v>
+        <v>113</v>
       </c>
       <c r="I11" t="s">
-        <v>156</v>
+        <v>124</v>
       </c>
       <c r="J11">
-        <v>430145000</v>
+        <v>1091123000</v>
       </c>
       <c r="K11">
-        <v>441843000</v>
+        <v>2516381000</v>
       </c>
       <c r="L11">
-        <v>191726000</v>
+        <v>-499300000</v>
       </c>
       <c r="M11">
-        <v>0</v>
+        <v>128345000</v>
       </c>
       <c r="N11">
-        <v>9568000</v>
+        <v>155662000</v>
       </c>
       <c r="O11">
-        <v>0</v>
+        <v>-339780000</v>
       </c>
       <c r="P11">
-        <v>-2994000</v>
+        <v>176623000</v>
       </c>
       <c r="Q11">
-        <v>0</v>
+        <v>351087000</v>
       </c>
       <c r="R11">
-        <v>-35928000</v>
+        <v>228389000</v>
       </c>
       <c r="S11">
-        <v>247019000</v>
+        <v>1186199000</v>
       </c>
       <c r="T11">
-        <v>1320301000</v>
+        <v>4578410000</v>
       </c>
       <c r="U11">
-        <v>-1204383000</v>
+        <v>-656415000</v>
       </c>
       <c r="V11">
         <v>0</v>
       </c>
       <c r="W11">
-        <v>0</v>
+        <v>-23922000</v>
       </c>
       <c r="X11">
         <v>0</v>
       </c>
       <c r="Y11">
-        <v>-64127000</v>
+        <v>-5079739000</v>
       </c>
       <c r="Z11">
-        <v>-1268510000</v>
+        <v>-5760076000</v>
       </c>
       <c r="AA11">
-        <v>0</v>
+        <v>-220000000</v>
       </c>
       <c r="AB11">
-        <v>35138000</v>
+        <v>0</v>
       </c>
       <c r="AC11">
-        <v>-21295000</v>
+        <v>-23922000</v>
       </c>
       <c r="AD11">
-        <v>-31294000</v>
+        <v>-167169000</v>
       </c>
       <c r="AE11">
-        <v>-39745000</v>
+        <v>1419630000</v>
       </c>
       <c r="AF11">
-        <v>-57196000</v>
+        <v>1008539000</v>
       </c>
       <c r="AG11">
-        <v>0</v>
+        <v>-5134000</v>
       </c>
       <c r="AH11">
-        <v>-5405000</v>
+        <v>442599000</v>
       </c>
       <c r="AI11">
-        <v>4443000</v>
+        <v>615726000</v>
       </c>
       <c r="AJ11">
-        <v>9848000</v>
+        <v>173127000</v>
       </c>
       <c r="AK11">
-        <v>1320301000</v>
+        <v>4578410000</v>
       </c>
       <c r="AL11">
-        <v>-1204383000</v>
+        <v>-656415000</v>
       </c>
       <c r="AM11">
-        <v>115918000</v>
+        <v>4578410000</v>
       </c>
       <c r="AN11" s="3" t="s">
-        <v>159</v>
+        <v>133</v>
       </c>
       <c r="AO11" s="3" t="s">
-        <v>180</v>
+        <v>152</v>
       </c>
     </row>
     <row r="12" spans="1:41">
@@ -2329,64 +2257,64 @@
         <v>51</v>
       </c>
       <c r="B12" s="2">
-        <v>38352</v>
+        <v>41274</v>
       </c>
       <c r="C12" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="D12" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="E12" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="F12" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="G12" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="H12" t="s">
-        <v>138</v>
+        <v>114</v>
       </c>
       <c r="I12" t="s">
-        <v>156</v>
+        <v>124</v>
       </c>
       <c r="J12">
-        <v>624855000</v>
+        <v>570279000</v>
       </c>
       <c r="K12">
-        <v>504403000</v>
+        <v>0</v>
       </c>
       <c r="L12">
-        <v>204231000</v>
+        <v>292938000</v>
       </c>
       <c r="M12">
-        <v>0</v>
+        <v>127778000</v>
       </c>
       <c r="N12">
-        <v>-44929000</v>
+        <v>-282749000</v>
       </c>
       <c r="O12">
-        <v>0</v>
+        <v>-178683000</v>
       </c>
       <c r="P12">
-        <v>-17898000</v>
+        <v>-156762000</v>
       </c>
       <c r="Q12">
-        <v>0</v>
+        <v>-17150000</v>
       </c>
       <c r="R12">
-        <v>-28381000</v>
+        <v>74158000</v>
       </c>
       <c r="S12">
-        <v>155787000</v>
+        <v>4528531000</v>
       </c>
       <c r="T12">
-        <v>1444347000</v>
+        <v>5236777000</v>
       </c>
       <c r="U12">
-        <v>-1416684000</v>
+        <v>-7355116000</v>
       </c>
       <c r="V12">
         <v>0</v>
@@ -2398,55 +2326,55 @@
         <v>0</v>
       </c>
       <c r="Y12">
-        <v>19776000</v>
+        <v>1235853000</v>
       </c>
       <c r="Z12">
-        <v>-1396908000</v>
+        <v>-6119263000</v>
       </c>
       <c r="AA12">
-        <v>0</v>
+        <v>-2824000</v>
       </c>
       <c r="AB12">
-        <v>75510000</v>
+        <v>0</v>
       </c>
       <c r="AC12">
-        <v>-50000000</v>
+        <v>-58592000</v>
       </c>
       <c r="AD12">
-        <v>-37595000</v>
+        <v>-181080000</v>
       </c>
       <c r="AE12">
-        <v>-31153000</v>
+        <v>1382247000</v>
       </c>
       <c r="AF12">
-        <v>-43238000</v>
+        <v>1139751000</v>
       </c>
       <c r="AG12">
-        <v>12336000</v>
+        <v>3444000</v>
       </c>
       <c r="AH12">
-        <v>16537000</v>
+        <v>260709000</v>
       </c>
       <c r="AI12">
-        <v>20980000</v>
+        <v>876435000</v>
       </c>
       <c r="AJ12">
-        <v>4443000</v>
+        <v>615726000</v>
       </c>
       <c r="AK12">
-        <v>1444347000</v>
+        <v>5236777000</v>
       </c>
       <c r="AL12">
-        <v>-1416684000</v>
+        <v>-7355116000</v>
       </c>
       <c r="AM12">
-        <v>27663000</v>
+        <v>-2118339000</v>
       </c>
       <c r="AN12" s="3" t="s">
-        <v>160</v>
+        <v>134</v>
       </c>
       <c r="AO12" s="3" t="s">
-        <v>181</v>
+        <v>153</v>
       </c>
     </row>
     <row r="13" spans="1:41">
@@ -2454,64 +2382,64 @@
         <v>52</v>
       </c>
       <c r="B13" s="2">
-        <v>38717</v>
+        <v>41639</v>
       </c>
       <c r="C13" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="D13" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="E13" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="F13" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="G13" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="H13" t="s">
-        <v>139</v>
+        <v>115</v>
       </c>
       <c r="I13" t="s">
-        <v>156</v>
+        <v>124</v>
       </c>
       <c r="J13">
-        <v>1259576000</v>
+        <v>2197109000</v>
       </c>
       <c r="K13">
-        <v>654258000</v>
+        <v>0</v>
       </c>
       <c r="L13">
-        <v>270291000</v>
+        <v>874765000</v>
       </c>
       <c r="M13">
-        <v>0</v>
+        <v>134055000</v>
       </c>
       <c r="N13">
-        <v>-13640000</v>
+        <v>102322000</v>
       </c>
       <c r="O13">
-        <v>0</v>
+        <v>-23613000</v>
       </c>
       <c r="P13">
-        <v>-23085000</v>
+        <v>53402000</v>
       </c>
       <c r="Q13">
-        <v>0</v>
+        <v>178701000</v>
       </c>
       <c r="R13">
-        <v>-10347000</v>
+        <v>-51361000</v>
       </c>
       <c r="S13">
-        <v>198941000</v>
+        <v>4021163000</v>
       </c>
       <c r="T13">
-        <v>2369426000</v>
+        <v>7329414000</v>
       </c>
       <c r="U13">
-        <v>-1724763000</v>
+        <v>-7060627000</v>
       </c>
       <c r="V13">
         <v>0</v>
@@ -2523,55 +2451,55 @@
         <v>0</v>
       </c>
       <c r="Y13">
-        <v>46655000</v>
+        <v>745849000</v>
       </c>
       <c r="Z13">
-        <v>-1678108000</v>
+        <v>-6314778000</v>
       </c>
       <c r="AA13">
-        <v>0</v>
+        <v>-405780000</v>
       </c>
       <c r="AB13">
-        <v>64668000</v>
+        <v>0</v>
       </c>
       <c r="AC13">
-        <v>0</v>
+        <v>-63784000</v>
       </c>
       <c r="AD13">
-        <v>-42986000</v>
+        <v>-199178000</v>
       </c>
       <c r="AE13">
-        <v>-93992000</v>
+        <v>94816000</v>
       </c>
       <c r="AF13">
-        <v>-72310000</v>
+        <v>-573926000</v>
       </c>
       <c r="AG13">
-        <v>3823000</v>
+        <v>1064000</v>
       </c>
       <c r="AH13">
-        <v>622831000</v>
+        <v>441774000</v>
       </c>
       <c r="AI13">
-        <v>643811000</v>
+        <v>1318209000</v>
       </c>
       <c r="AJ13">
-        <v>20980000</v>
+        <v>876435000</v>
       </c>
       <c r="AK13">
-        <v>2369426000</v>
+        <v>7329414000</v>
       </c>
       <c r="AL13">
-        <v>-1724763000</v>
+        <v>-7060627000</v>
       </c>
       <c r="AM13">
-        <v>644663000</v>
+        <v>268787000</v>
       </c>
       <c r="AN13" s="3" t="s">
-        <v>161</v>
+        <v>135</v>
       </c>
       <c r="AO13" s="3" t="s">
-        <v>182</v>
+        <v>154</v>
       </c>
     </row>
     <row r="14" spans="1:41">
@@ -2579,64 +2507,64 @@
         <v>53</v>
       </c>
       <c r="B14" s="2">
-        <v>39082</v>
+        <v>42004</v>
       </c>
       <c r="C14" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="D14" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="E14" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="F14" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="G14" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="H14" t="s">
-        <v>140</v>
+        <v>116</v>
       </c>
       <c r="I14" t="s">
-        <v>156</v>
+        <v>124</v>
       </c>
       <c r="J14">
-        <v>1299885000</v>
+        <v>2915487000</v>
       </c>
       <c r="K14">
-        <v>817089000</v>
+        <v>0</v>
       </c>
       <c r="L14">
-        <v>385842000</v>
+        <v>1704946000</v>
       </c>
       <c r="M14">
-        <v>0</v>
+        <v>145086000</v>
       </c>
       <c r="N14">
-        <v>-45032000</v>
+        <v>440698000</v>
       </c>
       <c r="O14">
-        <v>0</v>
+        <v>84982000</v>
       </c>
       <c r="P14">
-        <v>-50370000</v>
+        <v>-161958000</v>
       </c>
       <c r="Q14">
-        <v>0</v>
+        <v>543630000</v>
       </c>
       <c r="R14">
-        <v>-120255000</v>
+        <v>-103414000</v>
       </c>
       <c r="S14">
-        <v>120769000</v>
+        <v>3442938000</v>
       </c>
       <c r="T14">
-        <v>2578553000</v>
+        <v>8649155000</v>
       </c>
       <c r="U14">
-        <v>-2819230000</v>
+        <v>-8246805000</v>
       </c>
       <c r="V14">
         <v>0</v>
@@ -2648,55 +2576,55 @@
         <v>0</v>
       </c>
       <c r="Y14">
-        <v>108857000</v>
+        <v>733240000</v>
       </c>
       <c r="Z14">
-        <v>-2710373000</v>
+        <v>-7513565000</v>
       </c>
       <c r="AA14">
-        <v>0</v>
+        <v>-505966000</v>
       </c>
       <c r="AB14">
-        <v>36033000</v>
+        <v>0</v>
       </c>
       <c r="AC14">
-        <v>-50199000</v>
+        <v>-127424000</v>
       </c>
       <c r="AD14">
-        <v>-60443000</v>
+        <v>-279695000</v>
       </c>
       <c r="AE14">
-        <v>-224273000</v>
+        <v>585351000</v>
       </c>
       <c r="AF14">
-        <v>-298882000</v>
+        <v>-327734000</v>
       </c>
       <c r="AG14">
-        <v>5146000</v>
+        <v>-38852000</v>
       </c>
       <c r="AH14">
-        <v>-425556000</v>
+        <v>769004000</v>
       </c>
       <c r="AI14">
-        <v>218255000</v>
+        <v>2087213000</v>
       </c>
       <c r="AJ14">
-        <v>643811000</v>
+        <v>1318209000</v>
       </c>
       <c r="AK14">
-        <v>2578553000</v>
+        <v>8649155000</v>
       </c>
       <c r="AL14">
-        <v>-2819230000</v>
+        <v>-8246805000</v>
       </c>
       <c r="AM14">
-        <v>-240677000</v>
+        <v>402350000</v>
       </c>
       <c r="AN14" s="3" t="s">
-        <v>162</v>
+        <v>136</v>
       </c>
       <c r="AO14" s="3" t="s">
-        <v>183</v>
+        <v>155</v>
       </c>
     </row>
     <row r="15" spans="1:41">
@@ -2704,124 +2632,124 @@
         <v>54</v>
       </c>
       <c r="B15" s="2">
-        <v>39447</v>
+        <v>42369</v>
       </c>
       <c r="C15" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="D15" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="E15" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="F15" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="G15" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="H15" t="s">
-        <v>141</v>
+        <v>117</v>
       </c>
       <c r="I15" t="s">
+        <v>124</v>
+      </c>
+      <c r="J15">
+        <v>-4524515000</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>-2482307000</v>
+      </c>
+      <c r="M15">
+        <v>130577000</v>
+      </c>
+      <c r="N15">
+        <v>-145884000</v>
+      </c>
+      <c r="O15">
+        <v>641412000</v>
+      </c>
+      <c r="P15">
+        <v>58450000</v>
+      </c>
+      <c r="Q15">
+        <v>-1409197000</v>
+      </c>
+      <c r="R15">
+        <v>499767000</v>
+      </c>
+      <c r="S15">
+        <v>10617294000</v>
+      </c>
+      <c r="T15">
+        <v>3595165000</v>
+      </c>
+      <c r="U15">
+        <v>-5013163000</v>
+      </c>
+      <c r="V15">
+        <v>0</v>
+      </c>
+      <c r="W15">
+        <v>0</v>
+      </c>
+      <c r="X15">
+        <v>0</v>
+      </c>
+      <c r="Y15">
+        <v>-307093000</v>
+      </c>
+      <c r="Z15">
+        <v>-5320256000</v>
+      </c>
+      <c r="AA15">
+        <v>-506156000</v>
+      </c>
+      <c r="AB15">
+        <v>0</v>
+      </c>
+      <c r="AC15">
+        <v>-48791000</v>
+      </c>
+      <c r="AD15">
+        <v>-367005000</v>
+      </c>
+      <c r="AE15">
+        <v>1292873000</v>
+      </c>
+      <c r="AF15">
+        <v>370921000</v>
+      </c>
+      <c r="AG15">
+        <v>-14537000</v>
+      </c>
+      <c r="AH15">
+        <v>-1368707000</v>
+      </c>
+      <c r="AI15">
+        <v>718506000</v>
+      </c>
+      <c r="AJ15">
+        <v>2087213000</v>
+      </c>
+      <c r="AK15">
+        <v>3595165000</v>
+      </c>
+      <c r="AL15">
+        <v>-5013163000</v>
+      </c>
+      <c r="AM15">
+        <v>-1417998000</v>
+      </c>
+      <c r="AN15" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="AO15" s="3" t="s">
         <v>156</v>
-      </c>
-      <c r="J15">
-        <v>1089918000</v>
-      </c>
-      <c r="K15">
-        <v>1065545000</v>
-      </c>
-      <c r="L15">
-        <v>426827000</v>
-      </c>
-      <c r="M15">
-        <v>0</v>
-      </c>
-      <c r="N15">
-        <v>109526000</v>
-      </c>
-      <c r="O15">
-        <v>0</v>
-      </c>
-      <c r="P15">
-        <v>9638000</v>
-      </c>
-      <c r="Q15">
-        <v>0</v>
-      </c>
-      <c r="R15">
-        <v>-3440000</v>
-      </c>
-      <c r="S15">
-        <v>201549000</v>
-      </c>
-      <c r="T15">
-        <v>2893365000</v>
-      </c>
-      <c r="U15">
-        <v>-3679062000</v>
-      </c>
-      <c r="V15">
-        <v>0</v>
-      </c>
-      <c r="W15">
-        <v>0</v>
-      </c>
-      <c r="X15">
-        <v>0</v>
-      </c>
-      <c r="Y15">
-        <v>223288000</v>
-      </c>
-      <c r="Z15">
-        <v>-3455774000</v>
-      </c>
-      <c r="AA15">
-        <v>0</v>
-      </c>
-      <c r="AB15">
-        <v>55320000</v>
-      </c>
-      <c r="AC15">
-        <v>-51197000</v>
-      </c>
-      <c r="AD15">
-        <v>-84020000</v>
-      </c>
-      <c r="AE15">
-        <v>473620000</v>
-      </c>
-      <c r="AF15">
-        <v>393723000</v>
-      </c>
-      <c r="AG15">
-        <v>4662000</v>
-      </c>
-      <c r="AH15">
-        <v>-164024000</v>
-      </c>
-      <c r="AI15">
-        <v>54231000</v>
-      </c>
-      <c r="AJ15">
-        <v>218255000</v>
-      </c>
-      <c r="AK15">
-        <v>2893365000</v>
-      </c>
-      <c r="AL15">
-        <v>-3679062000</v>
-      </c>
-      <c r="AM15">
-        <v>-785697000</v>
-      </c>
-      <c r="AN15" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="AO15" s="3" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="16" spans="1:41">
@@ -2829,67 +2757,67 @@
         <v>55</v>
       </c>
       <c r="B16" s="2">
-        <v>39813</v>
+        <v>42735</v>
       </c>
       <c r="C16" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="D16" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="E16" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="F16" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G16" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="H16" t="s">
-        <v>142</v>
+        <v>118</v>
       </c>
       <c r="I16" t="s">
-        <v>156</v>
+        <v>124</v>
       </c>
       <c r="J16">
-        <v>2436919000</v>
+        <v>-1096686000</v>
       </c>
       <c r="K16">
-        <v>1326875000</v>
+        <v>0</v>
       </c>
       <c r="L16">
-        <v>1133630000</v>
+        <v>-515206000</v>
       </c>
       <c r="M16">
-        <v>0</v>
+        <v>128090000</v>
       </c>
       <c r="N16">
-        <v>97736000</v>
+        <v>-256334000</v>
       </c>
       <c r="O16">
-        <v>0</v>
+        <v>-232799000</v>
       </c>
       <c r="P16">
-        <v>-92049000</v>
+        <v>170694000</v>
       </c>
       <c r="Q16">
-        <v>0</v>
+        <v>-74048000</v>
       </c>
       <c r="R16">
-        <v>-1654000</v>
+        <v>-156102000</v>
       </c>
       <c r="S16">
-        <v>-361911000</v>
+        <v>4099199000</v>
       </c>
       <c r="T16">
-        <v>4633249000</v>
+        <v>2359063000</v>
       </c>
       <c r="U16">
-        <v>-5195471000</v>
+        <v>-2582795000</v>
       </c>
       <c r="V16">
-        <v>0</v>
+        <v>54534000</v>
       </c>
       <c r="W16">
         <v>0</v>
@@ -2898,55 +2826,55 @@
         <v>0</v>
       </c>
       <c r="Y16">
-        <v>228953000</v>
+        <v>1275317000</v>
       </c>
       <c r="Z16">
-        <v>-4966518000</v>
+        <v>-1252944000</v>
       </c>
       <c r="AA16">
-        <v>0</v>
+        <v>-570182000</v>
       </c>
       <c r="AB16">
-        <v>72572000</v>
+        <v>0</v>
       </c>
       <c r="AC16">
-        <v>-23229000</v>
+        <v>-82125000</v>
       </c>
       <c r="AD16">
-        <v>-115204000</v>
+        <v>-372845000</v>
       </c>
       <c r="AE16">
-        <v>710966000</v>
+        <v>782430000</v>
       </c>
       <c r="AF16">
-        <v>645105000</v>
+        <v>-242722000</v>
       </c>
       <c r="AG16">
-        <v>-34756000</v>
+        <v>17992000</v>
       </c>
       <c r="AH16">
-        <v>277080000</v>
+        <v>881389000</v>
       </c>
       <c r="AI16">
-        <v>331311000</v>
+        <v>1599895000</v>
       </c>
       <c r="AJ16">
-        <v>54231000</v>
+        <v>718506000</v>
       </c>
       <c r="AK16">
-        <v>4633249000</v>
+        <v>2359063000</v>
       </c>
       <c r="AL16">
-        <v>-5195471000</v>
+        <v>-2582795000</v>
       </c>
       <c r="AM16">
-        <v>-562222000</v>
+        <v>-223732000</v>
       </c>
       <c r="AN16" s="3" t="s">
-        <v>164</v>
+        <v>138</v>
       </c>
       <c r="AO16" s="3" t="s">
-        <v>185</v>
+        <v>157</v>
       </c>
     </row>
     <row r="17" spans="1:41">
@@ -2954,124 +2882,124 @@
         <v>56</v>
       </c>
       <c r="B17" s="2">
-        <v>40178</v>
+        <v>43100</v>
       </c>
       <c r="C17" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="D17" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="E17" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="F17" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="G17" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="H17" t="s">
-        <v>143</v>
+        <v>119</v>
       </c>
       <c r="I17" t="s">
-        <v>156</v>
+        <v>124</v>
       </c>
       <c r="J17">
-        <v>546627000</v>
+        <v>2582579000</v>
       </c>
       <c r="K17">
         <v>0</v>
       </c>
       <c r="L17">
-        <v>174392000</v>
+        <v>-1473872000</v>
       </c>
       <c r="M17">
-        <v>95180000</v>
+        <v>133849000</v>
       </c>
       <c r="N17">
-        <v>-178420000</v>
+        <v>-964912000</v>
       </c>
       <c r="O17">
-        <v>-47818000</v>
+        <v>-392131000</v>
       </c>
       <c r="P17">
-        <v>-50146000</v>
+        <v>-174548000</v>
       </c>
       <c r="Q17">
-        <v>-153565000</v>
+        <v>324192000</v>
       </c>
       <c r="R17">
-        <v>-17820000</v>
+        <v>89992000</v>
       </c>
       <c r="S17">
-        <v>2284660000</v>
+        <v>3987692000</v>
       </c>
       <c r="T17">
-        <v>2922439000</v>
+        <v>4265336000</v>
       </c>
       <c r="U17">
-        <v>-3503009000</v>
+        <v>-4124242000</v>
       </c>
       <c r="V17">
         <v>0</v>
       </c>
       <c r="W17">
-        <v>-118221000</v>
+        <v>0</v>
       </c>
       <c r="X17">
         <v>0</v>
       </c>
       <c r="Y17">
-        <v>206679000</v>
+        <v>136833000</v>
       </c>
       <c r="Z17">
-        <v>-3414551000</v>
+        <v>-3987409000</v>
       </c>
       <c r="AA17">
-        <v>0</v>
+        <v>-606555000</v>
       </c>
       <c r="AB17">
         <v>0</v>
       </c>
       <c r="AC17">
-        <v>-10986000</v>
+        <v>-63408000</v>
       </c>
       <c r="AD17">
-        <v>-142260000</v>
+        <v>-386531000</v>
       </c>
       <c r="AE17">
-        <v>987408000</v>
+        <v>20783000</v>
       </c>
       <c r="AF17">
-        <v>834162000</v>
+        <v>-1035711000</v>
       </c>
       <c r="AG17">
-        <v>12390000</v>
+        <v>-7883000</v>
       </c>
       <c r="AH17">
-        <v>354440000</v>
+        <v>-765667000</v>
       </c>
       <c r="AI17">
-        <v>685751000</v>
+        <v>834228000</v>
       </c>
       <c r="AJ17">
-        <v>331311000</v>
+        <v>1599895000</v>
       </c>
       <c r="AK17">
-        <v>2922439000</v>
+        <v>4265336000</v>
       </c>
       <c r="AL17">
-        <v>-3503009000</v>
+        <v>-4124242000</v>
       </c>
       <c r="AM17">
-        <v>-580570000</v>
+        <v>141094000</v>
       </c>
       <c r="AN17" s="3" t="s">
-        <v>165</v>
+        <v>139</v>
       </c>
       <c r="AO17" s="3" t="s">
-        <v>186</v>
+        <v>158</v>
       </c>
     </row>
     <row r="18" spans="1:41">
@@ -3079,67 +3007,67 @@
         <v>57</v>
       </c>
       <c r="B18" s="2">
-        <v>40543</v>
+        <v>43465</v>
       </c>
       <c r="C18" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="D18" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="E18" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="F18" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="G18" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="H18" t="s">
-        <v>144</v>
+        <v>120</v>
       </c>
       <c r="I18" t="s">
-        <v>156</v>
+        <v>124</v>
       </c>
       <c r="J18">
-        <v>160654000</v>
+        <v>3419040000</v>
       </c>
       <c r="K18">
         <v>0</v>
       </c>
       <c r="L18">
-        <v>76245000</v>
+        <v>894156000</v>
       </c>
       <c r="M18">
-        <v>107378000</v>
+        <v>155337000</v>
       </c>
       <c r="N18">
-        <v>-131122000</v>
+        <v>-230105000</v>
       </c>
       <c r="O18">
-        <v>-339126000</v>
+        <v>-368180000</v>
       </c>
       <c r="P18">
-        <v>-171791000</v>
+        <v>-395408000</v>
       </c>
       <c r="Q18">
-        <v>654688000</v>
+        <v>439347000</v>
       </c>
       <c r="R18">
-        <v>-221795000</v>
+        <v>301083000</v>
       </c>
       <c r="S18">
-        <v>2495447000</v>
+        <v>3530180000</v>
       </c>
       <c r="T18">
-        <v>2708602000</v>
+        <v>7768608000</v>
       </c>
       <c r="U18">
-        <v>-5581382000</v>
+        <v>-6076475000</v>
       </c>
       <c r="V18">
-        <v>-210000000</v>
+        <v>0</v>
       </c>
       <c r="W18">
         <v>0</v>
@@ -3148,55 +3076,55 @@
         <v>0</v>
       </c>
       <c r="Y18">
-        <v>888608000</v>
+        <v>-93687000</v>
       </c>
       <c r="Z18">
-        <v>-4902774000</v>
+        <v>-6170162000</v>
       </c>
       <c r="AA18">
-        <v>-45300000</v>
+        <v>-358219000</v>
       </c>
       <c r="AB18">
         <v>0</v>
       </c>
       <c r="AC18">
-        <v>-11295000</v>
+        <v>-63456000</v>
       </c>
       <c r="AD18">
-        <v>-153240000</v>
+        <v>-438045000</v>
       </c>
       <c r="AE18">
-        <v>2513254000</v>
+        <v>20617000</v>
       </c>
       <c r="AF18">
-        <v>2303419000</v>
+        <v>-839103000</v>
       </c>
       <c r="AG18">
-        <v>-6145000</v>
+        <v>-37937000</v>
       </c>
       <c r="AH18">
-        <v>103102000</v>
+        <v>721406000</v>
       </c>
       <c r="AI18">
-        <v>788853000</v>
+        <v>1555634000</v>
       </c>
       <c r="AJ18">
-        <v>685751000</v>
+        <v>834228000</v>
       </c>
       <c r="AK18">
-        <v>2708602000</v>
+        <v>7768608000</v>
       </c>
       <c r="AL18">
-        <v>-5581382000</v>
+        <v>-6076475000</v>
       </c>
       <c r="AM18">
-        <v>-2872780000</v>
+        <v>1692133000</v>
       </c>
       <c r="AN18" s="3" t="s">
-        <v>166</v>
+        <v>140</v>
       </c>
       <c r="AO18" s="3" t="s">
-        <v>187</v>
+        <v>159</v>
       </c>
     </row>
     <row r="19" spans="1:41">
@@ -3204,124 +3132,124 @@
         <v>58</v>
       </c>
       <c r="B19" s="2">
-        <v>40907</v>
+        <v>43830</v>
       </c>
       <c r="C19" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="D19" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="E19" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="F19" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="G19" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="H19" t="s">
-        <v>145</v>
+        <v>121</v>
       </c>
       <c r="I19" t="s">
-        <v>156</v>
+        <v>124</v>
       </c>
       <c r="J19">
-        <v>1091123000</v>
+        <v>2734910000</v>
       </c>
       <c r="K19">
-        <v>2516381000</v>
+        <v>0</v>
       </c>
       <c r="L19">
-        <v>-499300000</v>
+        <v>631658000</v>
       </c>
       <c r="M19">
-        <v>128345000</v>
+        <v>174738000</v>
       </c>
       <c r="N19">
-        <v>155662000</v>
+        <v>393474000</v>
       </c>
       <c r="O19">
-        <v>-339780000</v>
+        <v>-91792000</v>
       </c>
       <c r="P19">
-        <v>176623000</v>
+        <v>90284000</v>
       </c>
       <c r="Q19">
-        <v>351087000</v>
+        <v>168539000</v>
       </c>
       <c r="R19">
-        <v>228389000</v>
+        <v>-115061000</v>
       </c>
       <c r="S19">
-        <v>1186199000</v>
+        <v>4228400000</v>
       </c>
       <c r="T19">
-        <v>4578410000</v>
+        <v>8163180000</v>
       </c>
       <c r="U19">
-        <v>-656415000</v>
+        <v>-6422526000</v>
       </c>
       <c r="V19">
         <v>0</v>
       </c>
       <c r="W19">
-        <v>-23922000</v>
+        <v>0</v>
       </c>
       <c r="X19">
         <v>0</v>
       </c>
       <c r="Y19">
-        <v>-5079739000</v>
+        <v>245353000</v>
       </c>
       <c r="Z19">
-        <v>-5760076000</v>
+        <v>-6177173000</v>
       </c>
       <c r="AA19">
-        <v>-220000000</v>
+        <v>-912899000</v>
       </c>
       <c r="AB19">
         <v>0</v>
       </c>
       <c r="AC19">
-        <v>-23922000</v>
+        <v>-25152000</v>
       </c>
       <c r="AD19">
-        <v>-167169000</v>
+        <v>-588200000</v>
       </c>
       <c r="AE19">
-        <v>1419630000</v>
+        <v>12930000</v>
       </c>
       <c r="AF19">
-        <v>1008539000</v>
+        <v>-1513321000</v>
       </c>
       <c r="AG19">
-        <v>-5134000</v>
+        <v>-348000</v>
       </c>
       <c r="AH19">
-        <v>442599000</v>
+        <v>472338000</v>
       </c>
       <c r="AI19">
-        <v>615726000</v>
+        <v>2027972000</v>
       </c>
       <c r="AJ19">
-        <v>173127000</v>
+        <v>1555634000</v>
       </c>
       <c r="AK19">
-        <v>4578410000</v>
+        <v>8163180000</v>
       </c>
       <c r="AL19">
-        <v>-656415000</v>
+        <v>-6422526000</v>
       </c>
       <c r="AM19">
-        <v>4578410000</v>
+        <v>1740654000</v>
       </c>
       <c r="AN19" s="3" t="s">
-        <v>167</v>
+        <v>141</v>
       </c>
       <c r="AO19" s="3" t="s">
-        <v>188</v>
+        <v>160</v>
       </c>
     </row>
     <row r="20" spans="1:41">
@@ -3329,64 +3257,64 @@
         <v>59</v>
       </c>
       <c r="B20" s="2">
-        <v>41274</v>
+        <v>44196</v>
       </c>
       <c r="C20" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="D20" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="E20" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="F20" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="G20" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="H20" t="s">
-        <v>146</v>
+        <v>122</v>
       </c>
       <c r="I20" t="s">
-        <v>156</v>
+        <v>124</v>
       </c>
       <c r="J20">
-        <v>570279000</v>
+        <v>-604572000</v>
       </c>
       <c r="K20">
-        <v>0</v>
+        <v>-40673000000</v>
       </c>
       <c r="L20">
-        <v>292938000</v>
+        <v>-186390000</v>
       </c>
       <c r="M20">
-        <v>127778000</v>
+        <v>146396000</v>
       </c>
       <c r="N20">
-        <v>-282749000</v>
+        <v>152160000</v>
       </c>
       <c r="O20">
-        <v>-178683000</v>
+        <v>466523000</v>
       </c>
       <c r="P20">
-        <v>-156762000</v>
+        <v>122647000</v>
       </c>
       <c r="Q20">
-        <v>-17150000</v>
+        <v>-795267000</v>
       </c>
       <c r="R20">
-        <v>74158000</v>
+        <v>74734000</v>
       </c>
       <c r="S20">
-        <v>4528531000</v>
+        <v>46173189000</v>
       </c>
       <c r="T20">
-        <v>5236777000</v>
+        <v>5007783000</v>
       </c>
       <c r="U20">
-        <v>-7355116000</v>
+        <v>-3464700000</v>
       </c>
       <c r="V20">
         <v>0</v>
@@ -3398,55 +3326,55 @@
         <v>0</v>
       </c>
       <c r="Y20">
-        <v>1235853000</v>
+        <v>117194000</v>
       </c>
       <c r="Z20">
-        <v>-6119263000</v>
+        <v>-3347506000</v>
       </c>
       <c r="AA20">
-        <v>-2824000</v>
+        <v>-1019444000</v>
       </c>
       <c r="AB20">
-        <v>0</v>
+        <v>206000000</v>
       </c>
       <c r="AC20">
-        <v>-58592000</v>
+        <v>-16130000</v>
       </c>
       <c r="AD20">
-        <v>-181080000</v>
+        <v>-820823000</v>
       </c>
       <c r="AE20">
-        <v>1382247000</v>
+        <v>1291372000</v>
       </c>
       <c r="AF20">
-        <v>1139751000</v>
+        <v>-359025000</v>
       </c>
       <c r="AG20">
-        <v>3444000</v>
+        <v>-296000</v>
       </c>
       <c r="AH20">
-        <v>260709000</v>
+        <v>1300956000</v>
       </c>
       <c r="AI20">
-        <v>876435000</v>
+        <v>3328928000</v>
       </c>
       <c r="AJ20">
-        <v>615726000</v>
+        <v>2027972000</v>
       </c>
       <c r="AK20">
-        <v>5236777000</v>
+        <v>5007783000</v>
       </c>
       <c r="AL20">
-        <v>-7355116000</v>
+        <v>-3464700000</v>
       </c>
       <c r="AM20">
-        <v>-2118339000</v>
+        <v>1543083000</v>
       </c>
       <c r="AN20" s="3" t="s">
-        <v>168</v>
+        <v>142</v>
       </c>
       <c r="AO20" s="3" t="s">
-        <v>189</v>
+        <v>161</v>
       </c>
     </row>
     <row r="21" spans="1:41">
@@ -3454,64 +3382,64 @@
         <v>60</v>
       </c>
       <c r="B21" s="2">
-        <v>41639</v>
+        <v>44561</v>
       </c>
       <c r="C21" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="D21" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="E21" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="F21" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="G21" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="H21" t="s">
-        <v>147</v>
+        <v>123</v>
       </c>
       <c r="I21" t="s">
-        <v>156</v>
+        <v>124</v>
       </c>
       <c r="J21">
-        <v>2197109000</v>
+        <v>4664000000</v>
       </c>
       <c r="K21">
         <v>0</v>
       </c>
       <c r="L21">
-        <v>874765000</v>
+        <v>-122000000</v>
       </c>
       <c r="M21">
-        <v>134055000</v>
+        <v>152000000</v>
       </c>
       <c r="N21">
-        <v>102322000</v>
+        <v>-518000000</v>
       </c>
       <c r="O21">
-        <v>-23613000</v>
+        <v>-821000000</v>
       </c>
       <c r="P21">
-        <v>53402000</v>
+        <v>-13000000</v>
       </c>
       <c r="Q21">
-        <v>178701000</v>
+        <v>456000000</v>
       </c>
       <c r="R21">
-        <v>-51361000</v>
+        <v>-200000000</v>
       </c>
       <c r="S21">
-        <v>4021163000</v>
+        <v>4615000000</v>
       </c>
       <c r="T21">
-        <v>7329414000</v>
+        <v>8791000000</v>
       </c>
       <c r="U21">
-        <v>-7060627000</v>
+        <v>-3850000000</v>
       </c>
       <c r="V21">
         <v>0</v>
@@ -3523,1101 +3451,97 @@
         <v>0</v>
       </c>
       <c r="Y21">
-        <v>745849000</v>
+        <v>431000000</v>
       </c>
       <c r="Z21">
-        <v>-6314778000</v>
+        <v>-3419000000</v>
       </c>
       <c r="AA21">
-        <v>-405780000</v>
+        <v>-787000000</v>
       </c>
       <c r="AB21">
         <v>0</v>
       </c>
       <c r="AC21">
-        <v>-63784000</v>
+        <v>-41000000</v>
       </c>
       <c r="AD21">
-        <v>-199178000</v>
+        <v>-2684000000</v>
       </c>
       <c r="AE21">
-        <v>94816000</v>
+        <v>19000000</v>
       </c>
       <c r="AF21">
-        <v>-573926000</v>
+        <v>-3493000000</v>
       </c>
       <c r="AG21">
-        <v>1064000</v>
+        <v>1000000</v>
       </c>
       <c r="AH21">
-        <v>441774000</v>
+        <v>1880000000</v>
       </c>
       <c r="AI21">
-        <v>1318209000</v>
+        <v>5209000000</v>
       </c>
       <c r="AJ21">
-        <v>876435000</v>
+        <v>3329000000</v>
       </c>
       <c r="AK21">
-        <v>7329414000</v>
+        <v>8791000000</v>
       </c>
       <c r="AL21">
-        <v>-7060627000</v>
+        <v>-3850000000</v>
       </c>
       <c r="AM21">
-        <v>268787000</v>
+        <v>4941000000</v>
       </c>
       <c r="AN21" s="3" t="s">
-        <v>169</v>
+        <v>143</v>
       </c>
       <c r="AO21" s="3" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="22" spans="1:41">
-      <c r="A22" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B22" s="2">
-        <v>42004</v>
-      </c>
-      <c r="C22" t="s">
-        <v>69</v>
-      </c>
-      <c r="D22" t="s">
-        <v>70</v>
-      </c>
-      <c r="E22" t="s">
-        <v>71</v>
-      </c>
-      <c r="F22" t="s">
-        <v>92</v>
-      </c>
-      <c r="G22" t="s">
-        <v>120</v>
-      </c>
-      <c r="H22" t="s">
-        <v>148</v>
-      </c>
-      <c r="I22" t="s">
-        <v>156</v>
-      </c>
-      <c r="J22">
-        <v>2915487000</v>
-      </c>
-      <c r="K22">
-        <v>0</v>
-      </c>
-      <c r="L22">
-        <v>1704946000</v>
-      </c>
-      <c r="M22">
-        <v>145086000</v>
-      </c>
-      <c r="N22">
-        <v>440698000</v>
-      </c>
-      <c r="O22">
-        <v>84982000</v>
-      </c>
-      <c r="P22">
-        <v>-161958000</v>
-      </c>
-      <c r="Q22">
-        <v>543630000</v>
-      </c>
-      <c r="R22">
-        <v>-103414000</v>
-      </c>
-      <c r="S22">
-        <v>3442938000</v>
-      </c>
-      <c r="T22">
-        <v>8649155000</v>
-      </c>
-      <c r="U22">
-        <v>-8246805000</v>
-      </c>
-      <c r="V22">
-        <v>0</v>
-      </c>
-      <c r="W22">
-        <v>0</v>
-      </c>
-      <c r="X22">
-        <v>0</v>
-      </c>
-      <c r="Y22">
-        <v>733240000</v>
-      </c>
-      <c r="Z22">
-        <v>-7513565000</v>
-      </c>
-      <c r="AA22">
-        <v>-505966000</v>
-      </c>
-      <c r="AB22">
-        <v>0</v>
-      </c>
-      <c r="AC22">
-        <v>-127424000</v>
-      </c>
-      <c r="AD22">
-        <v>-279695000</v>
-      </c>
-      <c r="AE22">
-        <v>585351000</v>
-      </c>
-      <c r="AF22">
-        <v>-327734000</v>
-      </c>
-      <c r="AG22">
-        <v>-38852000</v>
-      </c>
-      <c r="AH22">
-        <v>769004000</v>
-      </c>
-      <c r="AI22">
-        <v>2087213000</v>
-      </c>
-      <c r="AJ22">
-        <v>1318209000</v>
-      </c>
-      <c r="AK22">
-        <v>8649155000</v>
-      </c>
-      <c r="AL22">
-        <v>-8246805000</v>
-      </c>
-      <c r="AM22">
-        <v>402350000</v>
-      </c>
-      <c r="AN22" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="AO22" s="3" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="23" spans="1:41">
-      <c r="A23" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B23" s="2">
-        <v>42369</v>
-      </c>
-      <c r="C23" t="s">
-        <v>69</v>
-      </c>
-      <c r="D23" t="s">
-        <v>70</v>
-      </c>
-      <c r="E23" t="s">
-        <v>71</v>
-      </c>
-      <c r="F23" t="s">
-        <v>93</v>
-      </c>
-      <c r="G23" t="s">
-        <v>121</v>
-      </c>
-      <c r="H23" t="s">
-        <v>149</v>
-      </c>
-      <c r="I23" t="s">
-        <v>156</v>
-      </c>
-      <c r="J23">
-        <v>-4524515000</v>
-      </c>
-      <c r="K23">
-        <v>0</v>
-      </c>
-      <c r="L23">
-        <v>-2482307000</v>
-      </c>
-      <c r="M23">
-        <v>130577000</v>
-      </c>
-      <c r="N23">
-        <v>-145884000</v>
-      </c>
-      <c r="O23">
-        <v>641412000</v>
-      </c>
-      <c r="P23">
-        <v>58450000</v>
-      </c>
-      <c r="Q23">
-        <v>-1409197000</v>
-      </c>
-      <c r="R23">
-        <v>499767000</v>
-      </c>
-      <c r="S23">
-        <v>10617294000</v>
-      </c>
-      <c r="T23">
-        <v>3595165000</v>
-      </c>
-      <c r="U23">
-        <v>-5013163000</v>
-      </c>
-      <c r="V23">
-        <v>0</v>
-      </c>
-      <c r="W23">
-        <v>0</v>
-      </c>
-      <c r="X23">
-        <v>0</v>
-      </c>
-      <c r="Y23">
-        <v>-307093000</v>
-      </c>
-      <c r="Z23">
-        <v>-5320256000</v>
-      </c>
-      <c r="AA23">
-        <v>-506156000</v>
-      </c>
-      <c r="AB23">
-        <v>0</v>
-      </c>
-      <c r="AC23">
-        <v>-48791000</v>
-      </c>
-      <c r="AD23">
-        <v>-367005000</v>
-      </c>
-      <c r="AE23">
-        <v>1292873000</v>
-      </c>
-      <c r="AF23">
-        <v>370921000</v>
-      </c>
-      <c r="AG23">
-        <v>-14537000</v>
-      </c>
-      <c r="AH23">
-        <v>-1368707000</v>
-      </c>
-      <c r="AI23">
-        <v>718506000</v>
-      </c>
-      <c r="AJ23">
-        <v>2087213000</v>
-      </c>
-      <c r="AK23">
-        <v>3595165000</v>
-      </c>
-      <c r="AL23">
-        <v>-5013163000</v>
-      </c>
-      <c r="AM23">
-        <v>-1417998000</v>
-      </c>
-      <c r="AN23" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="AO23" s="3" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="24" spans="1:41">
-      <c r="A24" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B24" s="2">
-        <v>42735</v>
-      </c>
-      <c r="C24" t="s">
-        <v>69</v>
-      </c>
-      <c r="D24" t="s">
-        <v>70</v>
-      </c>
-      <c r="E24" t="s">
-        <v>71</v>
-      </c>
-      <c r="F24" t="s">
-        <v>94</v>
-      </c>
-      <c r="G24" t="s">
-        <v>122</v>
-      </c>
-      <c r="H24" t="s">
-        <v>150</v>
-      </c>
-      <c r="I24" t="s">
-        <v>156</v>
-      </c>
-      <c r="J24">
-        <v>-1096686000</v>
-      </c>
-      <c r="K24">
-        <v>0</v>
-      </c>
-      <c r="L24">
-        <v>-515206000</v>
-      </c>
-      <c r="M24">
-        <v>128090000</v>
-      </c>
-      <c r="N24">
-        <v>-256334000</v>
-      </c>
-      <c r="O24">
-        <v>-232799000</v>
-      </c>
-      <c r="P24">
-        <v>170694000</v>
-      </c>
-      <c r="Q24">
-        <v>-74048000</v>
-      </c>
-      <c r="R24">
-        <v>-156102000</v>
-      </c>
-      <c r="S24">
-        <v>4099199000</v>
-      </c>
-      <c r="T24">
-        <v>2359063000</v>
-      </c>
-      <c r="U24">
-        <v>-2582795000</v>
-      </c>
-      <c r="V24">
-        <v>54534000</v>
-      </c>
-      <c r="W24">
-        <v>0</v>
-      </c>
-      <c r="X24">
-        <v>0</v>
-      </c>
-      <c r="Y24">
-        <v>1275317000</v>
-      </c>
-      <c r="Z24">
-        <v>-1252944000</v>
-      </c>
-      <c r="AA24">
-        <v>-570182000</v>
-      </c>
-      <c r="AB24">
-        <v>0</v>
-      </c>
-      <c r="AC24">
-        <v>-82125000</v>
-      </c>
-      <c r="AD24">
-        <v>-372845000</v>
-      </c>
-      <c r="AE24">
-        <v>782430000</v>
-      </c>
-      <c r="AF24">
-        <v>-242722000</v>
-      </c>
-      <c r="AG24">
-        <v>17992000</v>
-      </c>
-      <c r="AH24">
-        <v>881389000</v>
-      </c>
-      <c r="AI24">
-        <v>1599895000</v>
-      </c>
-      <c r="AJ24">
-        <v>718506000</v>
-      </c>
-      <c r="AK24">
-        <v>2359063000</v>
-      </c>
-      <c r="AL24">
-        <v>-2582795000</v>
-      </c>
-      <c r="AM24">
-        <v>-223732000</v>
-      </c>
-      <c r="AN24" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="AO24" s="3" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="25" spans="1:41">
-      <c r="A25" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B25" s="2">
-        <v>43100</v>
-      </c>
-      <c r="C25" t="s">
-        <v>69</v>
-      </c>
-      <c r="D25" t="s">
-        <v>70</v>
-      </c>
-      <c r="E25" t="s">
-        <v>71</v>
-      </c>
-      <c r="F25" t="s">
-        <v>95</v>
-      </c>
-      <c r="G25" t="s">
-        <v>123</v>
-      </c>
-      <c r="H25" t="s">
-        <v>151</v>
-      </c>
-      <c r="I25" t="s">
-        <v>156</v>
-      </c>
-      <c r="J25">
-        <v>2582579000</v>
-      </c>
-      <c r="K25">
-        <v>0</v>
-      </c>
-      <c r="L25">
-        <v>-1473872000</v>
-      </c>
-      <c r="M25">
-        <v>133849000</v>
-      </c>
-      <c r="N25">
-        <v>-964912000</v>
-      </c>
-      <c r="O25">
-        <v>-392131000</v>
-      </c>
-      <c r="P25">
-        <v>-174548000</v>
-      </c>
-      <c r="Q25">
-        <v>324192000</v>
-      </c>
-      <c r="R25">
-        <v>89992000</v>
-      </c>
-      <c r="S25">
-        <v>3987692000</v>
-      </c>
-      <c r="T25">
-        <v>4265336000</v>
-      </c>
-      <c r="U25">
-        <v>-4124242000</v>
-      </c>
-      <c r="V25">
-        <v>0</v>
-      </c>
-      <c r="W25">
-        <v>0</v>
-      </c>
-      <c r="X25">
-        <v>0</v>
-      </c>
-      <c r="Y25">
-        <v>136833000</v>
-      </c>
-      <c r="Z25">
-        <v>-3987409000</v>
-      </c>
-      <c r="AA25">
-        <v>-606555000</v>
-      </c>
-      <c r="AB25">
-        <v>0</v>
-      </c>
-      <c r="AC25">
-        <v>-63408000</v>
-      </c>
-      <c r="AD25">
-        <v>-386531000</v>
-      </c>
-      <c r="AE25">
-        <v>20783000</v>
-      </c>
-      <c r="AF25">
-        <v>-1035711000</v>
-      </c>
-      <c r="AG25">
-        <v>-7883000</v>
-      </c>
-      <c r="AH25">
-        <v>-765667000</v>
-      </c>
-      <c r="AI25">
-        <v>834228000</v>
-      </c>
-      <c r="AJ25">
-        <v>1599895000</v>
-      </c>
-      <c r="AK25">
-        <v>4265336000</v>
-      </c>
-      <c r="AL25">
-        <v>-4124242000</v>
-      </c>
-      <c r="AM25">
-        <v>141094000</v>
-      </c>
-      <c r="AN25" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="AO25" s="3" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="26" spans="1:41">
-      <c r="A26" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B26" s="2">
-        <v>43465</v>
-      </c>
-      <c r="C26" t="s">
-        <v>69</v>
-      </c>
-      <c r="D26" t="s">
-        <v>70</v>
-      </c>
-      <c r="E26" t="s">
-        <v>71</v>
-      </c>
-      <c r="F26" t="s">
-        <v>96</v>
-      </c>
-      <c r="G26" t="s">
-        <v>124</v>
-      </c>
-      <c r="H26" t="s">
-        <v>152</v>
-      </c>
-      <c r="I26" t="s">
-        <v>156</v>
-      </c>
-      <c r="J26">
-        <v>3419040000</v>
-      </c>
-      <c r="K26">
-        <v>0</v>
-      </c>
-      <c r="L26">
-        <v>894156000</v>
-      </c>
-      <c r="M26">
-        <v>155337000</v>
-      </c>
-      <c r="N26">
-        <v>-230105000</v>
-      </c>
-      <c r="O26">
-        <v>-368180000</v>
-      </c>
-      <c r="P26">
-        <v>-395408000</v>
-      </c>
-      <c r="Q26">
-        <v>439347000</v>
-      </c>
-      <c r="R26">
-        <v>301083000</v>
-      </c>
-      <c r="S26">
-        <v>3530180000</v>
-      </c>
-      <c r="T26">
-        <v>7768608000</v>
-      </c>
-      <c r="U26">
-        <v>-6076475000</v>
-      </c>
-      <c r="V26">
-        <v>0</v>
-      </c>
-      <c r="W26">
-        <v>0</v>
-      </c>
-      <c r="X26">
-        <v>0</v>
-      </c>
-      <c r="Y26">
-        <v>-93687000</v>
-      </c>
-      <c r="Z26">
-        <v>-6170162000</v>
-      </c>
-      <c r="AA26">
-        <v>-358219000</v>
-      </c>
-      <c r="AB26">
-        <v>0</v>
-      </c>
-      <c r="AC26">
-        <v>-63456000</v>
-      </c>
-      <c r="AD26">
-        <v>-438045000</v>
-      </c>
-      <c r="AE26">
-        <v>20617000</v>
-      </c>
-      <c r="AF26">
-        <v>-839103000</v>
-      </c>
-      <c r="AG26">
-        <v>-37937000</v>
-      </c>
-      <c r="AH26">
-        <v>721406000</v>
-      </c>
-      <c r="AI26">
-        <v>1555634000</v>
-      </c>
-      <c r="AJ26">
-        <v>834228000</v>
-      </c>
-      <c r="AK26">
-        <v>7768608000</v>
-      </c>
-      <c r="AL26">
-        <v>-6076475000</v>
-      </c>
-      <c r="AM26">
-        <v>1692133000</v>
-      </c>
-      <c r="AN26" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="AO26" s="3" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="27" spans="1:41">
-      <c r="A27" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B27" s="2">
-        <v>43830</v>
-      </c>
-      <c r="C27" t="s">
-        <v>69</v>
-      </c>
-      <c r="D27" t="s">
-        <v>70</v>
-      </c>
-      <c r="E27" t="s">
-        <v>71</v>
-      </c>
-      <c r="F27" t="s">
-        <v>97</v>
-      </c>
-      <c r="G27" t="s">
-        <v>125</v>
-      </c>
-      <c r="H27" t="s">
-        <v>153</v>
-      </c>
-      <c r="I27" t="s">
-        <v>156</v>
-      </c>
-      <c r="J27">
-        <v>2734910000</v>
-      </c>
-      <c r="K27">
-        <v>0</v>
-      </c>
-      <c r="L27">
-        <v>631658000</v>
-      </c>
-      <c r="M27">
-        <v>174738000</v>
-      </c>
-      <c r="N27">
-        <v>393474000</v>
-      </c>
-      <c r="O27">
-        <v>-91792000</v>
-      </c>
-      <c r="P27">
-        <v>90284000</v>
-      </c>
-      <c r="Q27">
-        <v>168539000</v>
-      </c>
-      <c r="R27">
-        <v>-115061000</v>
-      </c>
-      <c r="S27">
-        <v>4228400000</v>
-      </c>
-      <c r="T27">
-        <v>8163180000</v>
-      </c>
-      <c r="U27">
-        <v>-6422526000</v>
-      </c>
-      <c r="V27">
-        <v>0</v>
-      </c>
-      <c r="W27">
-        <v>0</v>
-      </c>
-      <c r="X27">
-        <v>0</v>
-      </c>
-      <c r="Y27">
-        <v>245353000</v>
-      </c>
-      <c r="Z27">
-        <v>-6177173000</v>
-      </c>
-      <c r="AA27">
-        <v>-912899000</v>
-      </c>
-      <c r="AB27">
-        <v>0</v>
-      </c>
-      <c r="AC27">
-        <v>-25152000</v>
-      </c>
-      <c r="AD27">
-        <v>-588200000</v>
-      </c>
-      <c r="AE27">
-        <v>12930000</v>
-      </c>
-      <c r="AF27">
-        <v>-1513321000</v>
-      </c>
-      <c r="AG27">
-        <v>-348000</v>
-      </c>
-      <c r="AH27">
-        <v>472338000</v>
-      </c>
-      <c r="AI27">
-        <v>2027972000</v>
-      </c>
-      <c r="AJ27">
-        <v>1555634000</v>
-      </c>
-      <c r="AK27">
-        <v>8163180000</v>
-      </c>
-      <c r="AL27">
-        <v>-6422526000</v>
-      </c>
-      <c r="AM27">
-        <v>1740654000</v>
-      </c>
-      <c r="AN27" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="AO27" s="3" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="28" spans="1:41">
-      <c r="A28" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B28" s="2">
-        <v>44196</v>
-      </c>
-      <c r="C28" t="s">
-        <v>69</v>
-      </c>
-      <c r="D28" t="s">
-        <v>70</v>
-      </c>
-      <c r="E28" t="s">
-        <v>71</v>
-      </c>
-      <c r="F28" t="s">
-        <v>98</v>
-      </c>
-      <c r="G28" t="s">
-        <v>126</v>
-      </c>
-      <c r="H28" t="s">
-        <v>154</v>
-      </c>
-      <c r="I28" t="s">
-        <v>156</v>
-      </c>
-      <c r="J28">
-        <v>-604572000</v>
-      </c>
-      <c r="K28">
-        <v>-40673000000</v>
-      </c>
-      <c r="L28">
-        <v>-186390000</v>
-      </c>
-      <c r="M28">
-        <v>146396000</v>
-      </c>
-      <c r="N28">
-        <v>152160000</v>
-      </c>
-      <c r="O28">
-        <v>466523000</v>
-      </c>
-      <c r="P28">
-        <v>122647000</v>
-      </c>
-      <c r="Q28">
-        <v>-795267000</v>
-      </c>
-      <c r="R28">
-        <v>74734000</v>
-      </c>
-      <c r="S28">
-        <v>46173189000</v>
-      </c>
-      <c r="T28">
-        <v>5007783000</v>
-      </c>
-      <c r="U28">
-        <v>-3464700000</v>
-      </c>
-      <c r="V28">
-        <v>0</v>
-      </c>
-      <c r="W28">
-        <v>0</v>
-      </c>
-      <c r="X28">
-        <v>0</v>
-      </c>
-      <c r="Y28">
-        <v>117194000</v>
-      </c>
-      <c r="Z28">
-        <v>-3347506000</v>
-      </c>
-      <c r="AA28">
-        <v>-1019444000</v>
-      </c>
-      <c r="AB28">
-        <v>206000000</v>
-      </c>
-      <c r="AC28">
-        <v>-16130000</v>
-      </c>
-      <c r="AD28">
-        <v>-820823000</v>
-      </c>
-      <c r="AE28">
-        <v>1291372000</v>
-      </c>
-      <c r="AF28">
-        <v>-359025000</v>
-      </c>
-      <c r="AG28">
-        <v>-296000</v>
-      </c>
-      <c r="AH28">
-        <v>1300956000</v>
-      </c>
-      <c r="AI28">
-        <v>3328928000</v>
-      </c>
-      <c r="AJ28">
-        <v>2027972000</v>
-      </c>
-      <c r="AK28">
-        <v>5007783000</v>
-      </c>
-      <c r="AL28">
-        <v>-3464700000</v>
-      </c>
-      <c r="AM28">
-        <v>1543083000</v>
-      </c>
-      <c r="AN28" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="AO28" s="3" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="29" spans="1:41">
-      <c r="A29" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B29" s="2">
-        <v>44561</v>
-      </c>
-      <c r="C29" t="s">
-        <v>69</v>
-      </c>
-      <c r="D29" t="s">
-        <v>70</v>
-      </c>
-      <c r="E29" t="s">
-        <v>71</v>
-      </c>
-      <c r="F29" t="s">
-        <v>99</v>
-      </c>
-      <c r="G29" t="s">
-        <v>127</v>
-      </c>
-      <c r="H29" t="s">
-        <v>155</v>
-      </c>
-      <c r="I29" t="s">
-        <v>156</v>
-      </c>
-      <c r="J29">
-        <v>4664000000</v>
-      </c>
-      <c r="K29">
-        <v>0</v>
-      </c>
-      <c r="L29">
-        <v>-122000000</v>
-      </c>
-      <c r="M29">
-        <v>152000000</v>
-      </c>
-      <c r="N29">
-        <v>-518000000</v>
-      </c>
-      <c r="O29">
-        <v>-821000000</v>
-      </c>
-      <c r="P29">
-        <v>-13000000</v>
-      </c>
-      <c r="Q29">
-        <v>456000000</v>
-      </c>
-      <c r="R29">
-        <v>-200000000</v>
-      </c>
-      <c r="S29">
-        <v>4615000000</v>
-      </c>
-      <c r="T29">
-        <v>8791000000</v>
-      </c>
-      <c r="U29">
-        <v>-3850000000</v>
-      </c>
-      <c r="V29">
-        <v>0</v>
-      </c>
-      <c r="W29">
-        <v>0</v>
-      </c>
-      <c r="X29">
-        <v>0</v>
-      </c>
-      <c r="Y29">
-        <v>431000000</v>
-      </c>
-      <c r="Z29">
-        <v>-3419000000</v>
-      </c>
-      <c r="AA29">
-        <v>-787000000</v>
-      </c>
-      <c r="AB29">
-        <v>0</v>
-      </c>
-      <c r="AC29">
-        <v>-41000000</v>
-      </c>
-      <c r="AD29">
-        <v>-2684000000</v>
-      </c>
-      <c r="AE29">
-        <v>19000000</v>
-      </c>
-      <c r="AF29">
-        <v>-3493000000</v>
-      </c>
-      <c r="AG29">
-        <v>1000000</v>
-      </c>
-      <c r="AH29">
-        <v>1880000000</v>
-      </c>
-      <c r="AI29">
-        <v>5209000000</v>
-      </c>
-      <c r="AJ29">
-        <v>3329000000</v>
-      </c>
-      <c r="AK29">
-        <v>8791000000</v>
-      </c>
-      <c r="AL29">
-        <v>-3850000000</v>
-      </c>
-      <c r="AM29">
-        <v>4941000000</v>
-      </c>
-      <c r="AN29" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="AO29" s="3" t="s">
-        <v>198</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="AN7" r:id="rId1"/>
-    <hyperlink ref="AO7" r:id="rId2"/>
-    <hyperlink ref="AN8" r:id="rId3"/>
-    <hyperlink ref="AO8" r:id="rId4"/>
-    <hyperlink ref="AN11" r:id="rId5"/>
-    <hyperlink ref="AO11" r:id="rId6"/>
-    <hyperlink ref="AN12" r:id="rId7"/>
-    <hyperlink ref="AO12" r:id="rId8"/>
-    <hyperlink ref="AN13" r:id="rId9"/>
-    <hyperlink ref="AO13" r:id="rId10"/>
-    <hyperlink ref="AN14" r:id="rId11"/>
-    <hyperlink ref="AO14" r:id="rId12"/>
-    <hyperlink ref="AN15" r:id="rId13"/>
-    <hyperlink ref="AO15" r:id="rId14"/>
-    <hyperlink ref="AN16" r:id="rId15"/>
-    <hyperlink ref="AO16" r:id="rId16"/>
-    <hyperlink ref="AN17" r:id="rId17"/>
-    <hyperlink ref="AO17" r:id="rId18"/>
-    <hyperlink ref="AN18" r:id="rId19"/>
-    <hyperlink ref="AO18" r:id="rId20"/>
-    <hyperlink ref="AN19" r:id="rId21"/>
-    <hyperlink ref="AO19" r:id="rId22"/>
-    <hyperlink ref="AN20" r:id="rId23"/>
-    <hyperlink ref="AO20" r:id="rId24"/>
-    <hyperlink ref="AN21" r:id="rId25"/>
-    <hyperlink ref="AO21" r:id="rId26"/>
-    <hyperlink ref="AN22" r:id="rId27"/>
-    <hyperlink ref="AO22" r:id="rId28"/>
-    <hyperlink ref="AN23" r:id="rId29"/>
-    <hyperlink ref="AO23" r:id="rId30"/>
-    <hyperlink ref="AN24" r:id="rId31"/>
-    <hyperlink ref="AO24" r:id="rId32"/>
-    <hyperlink ref="AN25" r:id="rId33"/>
-    <hyperlink ref="AO25" r:id="rId34"/>
-    <hyperlink ref="AN26" r:id="rId35"/>
-    <hyperlink ref="AO26" r:id="rId36"/>
-    <hyperlink ref="AN27" r:id="rId37"/>
-    <hyperlink ref="AO27" r:id="rId38"/>
-    <hyperlink ref="AN28" r:id="rId39"/>
-    <hyperlink ref="AO28" r:id="rId40"/>
-    <hyperlink ref="AN29" r:id="rId41"/>
-    <hyperlink ref="AO29" r:id="rId42"/>
+    <hyperlink ref="AN3" r:id="rId1"/>
+    <hyperlink ref="AO3" r:id="rId2"/>
+    <hyperlink ref="AN4" r:id="rId3"/>
+    <hyperlink ref="AO4" r:id="rId4"/>
+    <hyperlink ref="AN5" r:id="rId5"/>
+    <hyperlink ref="AO5" r:id="rId6"/>
+    <hyperlink ref="AN6" r:id="rId7"/>
+    <hyperlink ref="AO6" r:id="rId8"/>
+    <hyperlink ref="AN7" r:id="rId9"/>
+    <hyperlink ref="AO7" r:id="rId10"/>
+    <hyperlink ref="AN8" r:id="rId11"/>
+    <hyperlink ref="AO8" r:id="rId12"/>
+    <hyperlink ref="AN9" r:id="rId13"/>
+    <hyperlink ref="AO9" r:id="rId14"/>
+    <hyperlink ref="AN10" r:id="rId15"/>
+    <hyperlink ref="AO10" r:id="rId16"/>
+    <hyperlink ref="AN11" r:id="rId17"/>
+    <hyperlink ref="AO11" r:id="rId18"/>
+    <hyperlink ref="AN12" r:id="rId19"/>
+    <hyperlink ref="AO12" r:id="rId20"/>
+    <hyperlink ref="AN13" r:id="rId21"/>
+    <hyperlink ref="AO13" r:id="rId22"/>
+    <hyperlink ref="AN14" r:id="rId23"/>
+    <hyperlink ref="AO14" r:id="rId24"/>
+    <hyperlink ref="AN15" r:id="rId25"/>
+    <hyperlink ref="AO15" r:id="rId26"/>
+    <hyperlink ref="AN16" r:id="rId27"/>
+    <hyperlink ref="AO16" r:id="rId28"/>
+    <hyperlink ref="AN17" r:id="rId29"/>
+    <hyperlink ref="AO17" r:id="rId30"/>
+    <hyperlink ref="AN18" r:id="rId31"/>
+    <hyperlink ref="AO18" r:id="rId32"/>
+    <hyperlink ref="AN19" r:id="rId33"/>
+    <hyperlink ref="AO19" r:id="rId34"/>
+    <hyperlink ref="AN20" r:id="rId35"/>
+    <hyperlink ref="AO20" r:id="rId36"/>
+    <hyperlink ref="AN21" r:id="rId37"/>
+    <hyperlink ref="AO21" r:id="rId38"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>